<commit_message>
change format of 16/4
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2024.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2024.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Maart" sheetId="1" r:id="rId1"/>
@@ -487,7 +487,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -633,7 +633,6 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="6" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
@@ -1007,28 +1006,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
@@ -7516,8 +7515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L319"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="E137" sqref="E137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7534,28 +7533,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
@@ -10717,7 +10716,7 @@
       <c r="H146" s="30"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A147" s="44">
+      <c r="A147" s="23">
         <v>45398</v>
       </c>
       <c r="B147" s="24">
@@ -11433,7 +11432,7 @@
       <c r="D179" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E179" s="45">
+      <c r="E179" s="44">
         <v>0.18333333333333335</v>
       </c>
       <c r="F179" s="26" t="s">
@@ -14283,8 +14282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L319"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14295,7 +14294,7 @@
     <col min="4" max="4" width="2.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1796875" style="50" customWidth="1"/>
+    <col min="7" max="7" width="22.1796875" style="49" customWidth="1"/>
     <col min="8" max="8" width="30.26953125" style="1" customWidth="1"/>
     <col min="9" max="11" width="9.1796875" style="1"/>
     <col min="12" max="12" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
@@ -14303,28 +14302,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
@@ -14335,7 +14334,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="46"/>
+      <c r="G3" s="45"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -14353,7 +14352,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="6"/>
-      <c r="G4" s="47" t="s">
+      <c r="G4" s="46" t="s">
         <v>7</v>
       </c>
       <c r="H4" s="9" t="s">
@@ -14367,7 +14366,7 @@
       <c r="D5" s="12"/>
       <c r="E5" s="13"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="47" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="15"/>
@@ -14379,7 +14378,7 @@
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
       <c r="F6" s="19"/>
-      <c r="G6" s="49"/>
+      <c r="G6" s="48"/>
       <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -15464,7 +15463,7 @@
       <c r="G55" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H55" s="51" t="s">
+      <c r="H55" s="50" t="s">
         <v>62</v>
       </c>
     </row>
@@ -15977,7 +15976,7 @@
       <c r="H78" s="30"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A79" s="52">
+      <c r="A79" s="51">
         <v>45421</v>
       </c>
       <c r="B79" s="24">

</xml_diff>

<commit_message>
19 april should be one row lower
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2024.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2024.xlsx
@@ -7515,8 +7515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="E137" sqref="E137"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="C172" sqref="C172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11224,9 +11224,6 @@
       <c r="H169" s="41"/>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A170" s="23">
-        <v>45401</v>
-      </c>
       <c r="B170" s="24">
         <v>0.91666666666666663</v>
       </c>
@@ -11250,7 +11247,9 @@
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A171" s="23"/>
+      <c r="A171" s="23">
+        <v>45401</v>
+      </c>
       <c r="B171" s="24">
         <v>6.5972222222222224E-2</v>
       </c>

</xml_diff>

<commit_message>
10 mei 13:12 is wss 3:12
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2024.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2024.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Maart" sheetId="1" r:id="rId1"/>
@@ -7515,7 +7515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+    <sheetView topLeftCell="A163" workbookViewId="0">
       <selection activeCell="C172" sqref="C172"/>
     </sheetView>
   </sheetViews>
@@ -14281,8 +14281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L319"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16199,7 +16199,7 @@
         <v>45422</v>
       </c>
       <c r="B89" s="24">
-        <v>1.55</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="C89" s="25">
         <v>1.98</v>

</xml_diff>